<commit_message>
Fixes #1, Fixes #2, re-organize into modules
</commit_message>
<xml_diff>
--- a/data/bookings.xlsx
+++ b/data/bookings.xlsx
@@ -12,9 +12,10 @@
     <sheet name="2018-08" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="2018-09" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="2018-10" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Clients" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="Facilities" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="Rates" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="2018-11" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Clients" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Facilities" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Rates" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="69">
   <si>
     <t xml:space="preserve">First Floor Hall</t>
   </si>
@@ -239,10 +240,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="165" formatCode="YYYY/MM/DD"/>
     <numFmt numFmtId="166" formatCode="DDD"/>
+    <numFmt numFmtId="167" formatCode="YYYY/MM/DD"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -318,7 +320,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -336,6 +338,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -359,7 +365,7 @@
   <dimension ref="A1:T32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -427,101 +433,101 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
-        <v>43374</v>
+        <v>43282</v>
       </c>
       <c r="B2" s="3" t="n">
         <f aca="false">A2</f>
-        <v>43374</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43282</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
         <f aca="false">A2+1</f>
-        <v>43375</v>
+        <v>43283</v>
       </c>
       <c r="B3" s="3" t="n">
         <f aca="false">A3</f>
-        <v>43375</v>
+        <v>43283</v>
       </c>
       <c r="M3" s="0" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
         <f aca="false">A3+1</f>
-        <v>43376</v>
+        <v>43284</v>
       </c>
       <c r="B4" s="3" t="n">
         <f aca="false">A4</f>
-        <v>43376</v>
+        <v>43284</v>
       </c>
       <c r="M4" s="0" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
         <f aca="false">A4+1</f>
-        <v>43377</v>
+        <v>43285</v>
       </c>
       <c r="B5" s="3" t="n">
         <f aca="false">A5</f>
-        <v>43377</v>
+        <v>43285</v>
       </c>
       <c r="M5" s="0" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
         <f aca="false">A5+1</f>
-        <v>43378</v>
+        <v>43286</v>
       </c>
       <c r="B6" s="3" t="n">
         <f aca="false">A6</f>
-        <v>43378</v>
+        <v>43286</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
         <f aca="false">A6+1</f>
-        <v>43379</v>
+        <v>43287</v>
       </c>
       <c r="B7" s="3" t="n">
         <f aca="false">A7</f>
-        <v>43379</v>
+        <v>43287</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
         <f aca="false">A7+1</f>
-        <v>43380</v>
+        <v>43288</v>
       </c>
       <c r="B8" s="3" t="n">
         <f aca="false">A8</f>
-        <v>43380</v>
+        <v>43288</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="n">
         <f aca="false">A8+1</f>
-        <v>43381</v>
+        <v>43289</v>
       </c>
       <c r="B9" s="3" t="n">
         <f aca="false">A9</f>
-        <v>43381</v>
+        <v>43289</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>19</v>
@@ -530,50 +536,50 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="n">
         <f aca="false">A9+1</f>
-        <v>43382</v>
+        <v>43290</v>
       </c>
       <c r="B10" s="3" t="n">
         <f aca="false">A10</f>
-        <v>43382</v>
+        <v>43290</v>
       </c>
       <c r="N10" s="0" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="n">
         <f aca="false">A10+1</f>
-        <v>43383</v>
+        <v>43291</v>
       </c>
       <c r="B11" s="3" t="n">
         <f aca="false">A11</f>
-        <v>43383</v>
+        <v>43291</v>
       </c>
       <c r="P11" s="0" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="n">
         <f aca="false">A11+1</f>
-        <v>43384</v>
+        <v>43292</v>
       </c>
       <c r="B12" s="3" t="n">
         <f aca="false">A12</f>
-        <v>43384</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43292</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="n">
         <f aca="false">A12+1</f>
-        <v>43385</v>
+        <v>43293</v>
       </c>
       <c r="B13" s="3" t="n">
         <f aca="false">A13</f>
-        <v>43385</v>
+        <v>43293</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>18</v>
@@ -582,27 +588,27 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="n">
         <f aca="false">A13+1</f>
-        <v>43386</v>
+        <v>43294</v>
       </c>
       <c r="B14" s="3" t="n">
         <f aca="false">A14</f>
-        <v>43386</v>
+        <v>43294</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="n">
         <f aca="false">A14+1</f>
-        <v>43387</v>
+        <v>43295</v>
       </c>
       <c r="B15" s="3" t="n">
         <f aca="false">A15</f>
-        <v>43387</v>
+        <v>43295</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>18</v>
@@ -611,14 +617,14 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="n">
         <f aca="false">A15+1</f>
-        <v>43388</v>
+        <v>43296</v>
       </c>
       <c r="B16" s="3" t="n">
         <f aca="false">A16</f>
-        <v>43388</v>
+        <v>43296</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>18</v>
@@ -627,27 +633,27 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="n">
         <f aca="false">A16+1</f>
-        <v>43389</v>
+        <v>43297</v>
       </c>
       <c r="B17" s="3" t="n">
         <f aca="false">A17</f>
-        <v>43389</v>
+        <v>43297</v>
       </c>
       <c r="R17" s="0" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="n">
         <f aca="false">A17+1</f>
-        <v>43390</v>
+        <v>43298</v>
       </c>
       <c r="B18" s="3" t="n">
         <f aca="false">A18</f>
-        <v>43390</v>
+        <v>43298</v>
       </c>
       <c r="F18" s="0" t="s">
         <v>20</v>
@@ -656,53 +662,53 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="n">
         <f aca="false">A18+1</f>
-        <v>43391</v>
+        <v>43299</v>
       </c>
       <c r="B19" s="3" t="n">
         <f aca="false">A19</f>
-        <v>43391</v>
+        <v>43299</v>
       </c>
       <c r="F19" s="0" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="n">
         <f aca="false">A19+1</f>
-        <v>43392</v>
+        <v>43300</v>
       </c>
       <c r="B20" s="3" t="n">
         <f aca="false">A20</f>
-        <v>43392</v>
+        <v>43300</v>
       </c>
       <c r="F20" s="0" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="n">
         <f aca="false">A20+1</f>
-        <v>43393</v>
+        <v>43301</v>
       </c>
       <c r="B21" s="3" t="n">
         <f aca="false">A21</f>
-        <v>43393</v>
+        <v>43301</v>
       </c>
       <c r="O21" s="0" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="n">
         <f aca="false">A21+1</f>
-        <v>43394</v>
+        <v>43302</v>
       </c>
       <c r="B22" s="3" t="n">
         <f aca="false">A22</f>
-        <v>43394</v>
+        <v>43302</v>
       </c>
       <c r="I22" s="0" t="s">
         <v>20</v>
@@ -711,14 +717,14 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="n">
         <f aca="false">A22+1</f>
-        <v>43395</v>
+        <v>43303</v>
       </c>
       <c r="B23" s="3" t="n">
         <f aca="false">A23</f>
-        <v>43395</v>
+        <v>43303</v>
       </c>
       <c r="I23" s="0" t="s">
         <v>20</v>
@@ -727,14 +733,14 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="n">
         <f aca="false">A23+1</f>
-        <v>43396</v>
+        <v>43304</v>
       </c>
       <c r="B24" s="3" t="n">
         <f aca="false">A24</f>
-        <v>43396</v>
+        <v>43304</v>
       </c>
       <c r="O24" s="0" t="s">
         <v>18</v>
@@ -743,96 +749,96 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="n">
         <f aca="false">A24+1</f>
-        <v>43397</v>
+        <v>43305</v>
       </c>
       <c r="B25" s="3" t="n">
         <f aca="false">A25</f>
-        <v>43397</v>
+        <v>43305</v>
       </c>
       <c r="S25" s="0" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="n">
         <f aca="false">A25+1</f>
-        <v>43398</v>
+        <v>43306</v>
       </c>
       <c r="B26" s="3" t="n">
         <f aca="false">A26</f>
-        <v>43398</v>
+        <v>43306</v>
       </c>
       <c r="S26" s="0" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="n">
         <f aca="false">A26+1</f>
-        <v>43399</v>
+        <v>43307</v>
       </c>
       <c r="B27" s="3" t="n">
         <f aca="false">A27</f>
-        <v>43399</v>
+        <v>43307</v>
       </c>
       <c r="S27" s="0" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="n">
         <f aca="false">A27+1</f>
-        <v>43400</v>
+        <v>43308</v>
       </c>
       <c r="B28" s="3" t="n">
         <f aca="false">A28</f>
-        <v>43400</v>
+        <v>43308</v>
       </c>
       <c r="S28" s="0" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="n">
         <f aca="false">A28+1</f>
-        <v>43401</v>
+        <v>43309</v>
       </c>
       <c r="B29" s="3" t="n">
         <f aca="false">A29</f>
-        <v>43401</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43309</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="n">
         <f aca="false">A29+1</f>
-        <v>43402</v>
+        <v>43310</v>
       </c>
       <c r="B30" s="3" t="n">
         <f aca="false">A30</f>
-        <v>43402</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43310</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="n">
         <f aca="false">A30+1</f>
-        <v>43403</v>
+        <v>43311</v>
       </c>
       <c r="B31" s="3" t="n">
         <f aca="false">A31</f>
-        <v>43403</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43311</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="n">
         <f aca="false">A31+1</f>
-        <v>43404</v>
+        <v>43312</v>
       </c>
       <c r="B32" s="3" t="n">
         <f aca="false">A32</f>
-        <v>43404</v>
+        <v>43312</v>
       </c>
     </row>
   </sheetData>
@@ -854,7 +860,7 @@
   <dimension ref="A1:T32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -924,21 +930,21 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
-        <v>43374</v>
+        <v>43313</v>
       </c>
       <c r="B2" s="3" t="n">
         <f aca="false">A2</f>
-        <v>43374</v>
+        <v>43313</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
         <f aca="false">A2+1</f>
-        <v>43375</v>
+        <v>43314</v>
       </c>
       <c r="B3" s="3" t="n">
         <f aca="false">A3</f>
-        <v>43375</v>
+        <v>43314</v>
       </c>
       <c r="M3" s="0" t="s">
         <v>18</v>
@@ -947,11 +953,11 @@
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
         <f aca="false">A3+1</f>
-        <v>43376</v>
+        <v>43315</v>
       </c>
       <c r="B4" s="3" t="n">
         <f aca="false">A4</f>
-        <v>43376</v>
+        <v>43315</v>
       </c>
       <c r="M4" s="0" t="s">
         <v>18</v>
@@ -960,11 +966,11 @@
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
         <f aca="false">A4+1</f>
-        <v>43377</v>
+        <v>43316</v>
       </c>
       <c r="B5" s="3" t="n">
         <f aca="false">A5</f>
-        <v>43377</v>
+        <v>43316</v>
       </c>
       <c r="M5" s="0" t="s">
         <v>18</v>
@@ -973,11 +979,11 @@
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
         <f aca="false">A5+1</f>
-        <v>43378</v>
+        <v>43317</v>
       </c>
       <c r="B6" s="3" t="n">
         <f aca="false">A6</f>
-        <v>43378</v>
+        <v>43317</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>19</v>
@@ -986,11 +992,11 @@
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
         <f aca="false">A6+1</f>
-        <v>43379</v>
+        <v>43318</v>
       </c>
       <c r="B7" s="3" t="n">
         <f aca="false">A7</f>
-        <v>43379</v>
+        <v>43318</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>19</v>
@@ -1002,11 +1008,11 @@
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
         <f aca="false">A7+1</f>
-        <v>43380</v>
+        <v>43319</v>
       </c>
       <c r="B8" s="3" t="n">
         <f aca="false">A8</f>
-        <v>43380</v>
+        <v>43319</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>19</v>
@@ -1024,11 +1030,11 @@
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="n">
         <f aca="false">A8+1</f>
-        <v>43381</v>
+        <v>43320</v>
       </c>
       <c r="B9" s="3" t="n">
         <f aca="false">A9</f>
-        <v>43381</v>
+        <v>43320</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>19</v>
@@ -1049,11 +1055,11 @@
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="n">
         <f aca="false">A9+1</f>
-        <v>43382</v>
+        <v>43321</v>
       </c>
       <c r="B10" s="3" t="n">
         <f aca="false">A10</f>
-        <v>43382</v>
+        <v>43321</v>
       </c>
       <c r="N10" s="0" t="s">
         <v>19</v>
@@ -1065,11 +1071,11 @@
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="n">
         <f aca="false">A10+1</f>
-        <v>43383</v>
+        <v>43322</v>
       </c>
       <c r="B11" s="3" t="n">
         <f aca="false">A11</f>
-        <v>43383</v>
+        <v>43322</v>
       </c>
       <c r="H11" s="0" t="s">
         <v>21</v>
@@ -1081,21 +1087,21 @@
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="n">
         <f aca="false">A11+1</f>
-        <v>43384</v>
+        <v>43323</v>
       </c>
       <c r="B12" s="3" t="n">
         <f aca="false">A12</f>
-        <v>43384</v>
+        <v>43323</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="n">
         <f aca="false">A12+1</f>
-        <v>43385</v>
+        <v>43324</v>
       </c>
       <c r="B13" s="3" t="n">
         <f aca="false">A13</f>
-        <v>43385</v>
+        <v>43324</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>18</v>
@@ -1110,11 +1116,11 @@
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="n">
         <f aca="false">A13+1</f>
-        <v>43386</v>
+        <v>43325</v>
       </c>
       <c r="B14" s="3" t="n">
         <f aca="false">A14</f>
-        <v>43386</v>
+        <v>43325</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>18</v>
@@ -1123,11 +1129,11 @@
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="n">
         <f aca="false">A14+1</f>
-        <v>43387</v>
+        <v>43326</v>
       </c>
       <c r="B15" s="3" t="n">
         <f aca="false">A15</f>
-        <v>43387</v>
+        <v>43326</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>18</v>
@@ -1142,11 +1148,11 @@
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="n">
         <f aca="false">A15+1</f>
-        <v>43388</v>
+        <v>43327</v>
       </c>
       <c r="B16" s="3" t="n">
         <f aca="false">A16</f>
-        <v>43388</v>
+        <v>43327</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>18</v>
@@ -1161,11 +1167,11 @@
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="n">
         <f aca="false">A16+1</f>
-        <v>43389</v>
+        <v>43328</v>
       </c>
       <c r="B17" s="3" t="n">
         <f aca="false">A17</f>
-        <v>43389</v>
+        <v>43328</v>
       </c>
       <c r="O17" s="0" t="s">
         <v>21</v>
@@ -1177,11 +1183,11 @@
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="n">
         <f aca="false">A17+1</f>
-        <v>43390</v>
+        <v>43329</v>
       </c>
       <c r="B18" s="3" t="n">
         <f aca="false">A18</f>
-        <v>43390</v>
+        <v>43329</v>
       </c>
       <c r="F18" s="0" t="s">
         <v>20</v>
@@ -1196,11 +1202,11 @@
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="n">
         <f aca="false">A18+1</f>
-        <v>43391</v>
+        <v>43330</v>
       </c>
       <c r="B19" s="3" t="n">
         <f aca="false">A19</f>
-        <v>43391</v>
+        <v>43330</v>
       </c>
       <c r="F19" s="0" t="s">
         <v>20</v>
@@ -1209,11 +1215,11 @@
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="n">
         <f aca="false">A19+1</f>
-        <v>43392</v>
+        <v>43331</v>
       </c>
       <c r="B20" s="3" t="n">
         <f aca="false">A20</f>
-        <v>43392</v>
+        <v>43331</v>
       </c>
       <c r="F20" s="0" t="s">
         <v>20</v>
@@ -1222,11 +1228,11 @@
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="n">
         <f aca="false">A20+1</f>
-        <v>43393</v>
+        <v>43332</v>
       </c>
       <c r="B21" s="3" t="n">
         <f aca="false">A21</f>
-        <v>43393</v>
+        <v>43332</v>
       </c>
       <c r="O21" s="0" t="s">
         <v>18</v>
@@ -1235,11 +1241,11 @@
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="n">
         <f aca="false">A21+1</f>
-        <v>43394</v>
+        <v>43333</v>
       </c>
       <c r="B22" s="3" t="n">
         <f aca="false">A22</f>
-        <v>43394</v>
+        <v>43333</v>
       </c>
       <c r="I22" s="0" t="s">
         <v>20</v>
@@ -1251,11 +1257,11 @@
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="n">
         <f aca="false">A22+1</f>
-        <v>43395</v>
+        <v>43334</v>
       </c>
       <c r="B23" s="3" t="n">
         <f aca="false">A23</f>
-        <v>43395</v>
+        <v>43334</v>
       </c>
       <c r="I23" s="0" t="s">
         <v>20</v>
@@ -1267,11 +1273,11 @@
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="n">
         <f aca="false">A23+1</f>
-        <v>43396</v>
+        <v>43335</v>
       </c>
       <c r="B24" s="3" t="n">
         <f aca="false">A24</f>
-        <v>43396</v>
+        <v>43335</v>
       </c>
       <c r="O24" s="0" t="s">
         <v>18</v>
@@ -1283,11 +1289,11 @@
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="n">
         <f aca="false">A24+1</f>
-        <v>43397</v>
+        <v>43336</v>
       </c>
       <c r="B25" s="3" t="n">
         <f aca="false">A25</f>
-        <v>43397</v>
+        <v>43336</v>
       </c>
       <c r="S25" s="0" t="s">
         <v>20</v>
@@ -1296,11 +1302,11 @@
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="n">
         <f aca="false">A25+1</f>
-        <v>43398</v>
+        <v>43337</v>
       </c>
       <c r="B26" s="3" t="n">
         <f aca="false">A26</f>
-        <v>43398</v>
+        <v>43337</v>
       </c>
       <c r="S26" s="0" t="s">
         <v>20</v>
@@ -1309,11 +1315,11 @@
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="n">
         <f aca="false">A26+1</f>
-        <v>43399</v>
+        <v>43338</v>
       </c>
       <c r="B27" s="3" t="n">
         <f aca="false">A27</f>
-        <v>43399</v>
+        <v>43338</v>
       </c>
       <c r="S27" s="0" t="s">
         <v>20</v>
@@ -1322,11 +1328,11 @@
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="n">
         <f aca="false">A27+1</f>
-        <v>43400</v>
+        <v>43339</v>
       </c>
       <c r="B28" s="3" t="n">
         <f aca="false">A28</f>
-        <v>43400</v>
+        <v>43339</v>
       </c>
       <c r="S28" s="0" t="s">
         <v>20</v>
@@ -1335,41 +1341,41 @@
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="n">
         <f aca="false">A28+1</f>
-        <v>43401</v>
+        <v>43340</v>
       </c>
       <c r="B29" s="3" t="n">
         <f aca="false">A29</f>
-        <v>43401</v>
+        <v>43340</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="n">
         <f aca="false">A29+1</f>
-        <v>43402</v>
+        <v>43341</v>
       </c>
       <c r="B30" s="3" t="n">
         <f aca="false">A30</f>
-        <v>43402</v>
+        <v>43341</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="n">
         <f aca="false">A30+1</f>
-        <v>43403</v>
+        <v>43342</v>
       </c>
       <c r="B31" s="3" t="n">
         <f aca="false">A31</f>
-        <v>43403</v>
+        <v>43342</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="n">
         <f aca="false">A31+1</f>
-        <v>43404</v>
+        <v>43343</v>
       </c>
       <c r="B32" s="3" t="n">
         <f aca="false">A32</f>
-        <v>43404</v>
+        <v>43343</v>
       </c>
     </row>
   </sheetData>
@@ -1391,7 +1397,7 @@
   <dimension ref="A1:T32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L29" activeCellId="0" sqref="L29"/>
+      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1460,74 +1466,74 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="n">
-        <v>43374</v>
+      <c r="A2" s="5" t="n">
+        <v>43344</v>
       </c>
       <c r="B2" s="3" t="n">
         <f aca="false">A2</f>
-        <v>43374</v>
+        <v>43344</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="n">
+      <c r="A3" s="5" t="n">
         <f aca="false">A2+1</f>
-        <v>43375</v>
+        <v>43345</v>
       </c>
       <c r="B3" s="3" t="n">
         <f aca="false">A3</f>
-        <v>43375</v>
+        <v>43345</v>
       </c>
       <c r="M3" s="0" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="n">
+      <c r="A4" s="5" t="n">
         <f aca="false">A3+1</f>
-        <v>43376</v>
+        <v>43346</v>
       </c>
       <c r="B4" s="3" t="n">
         <f aca="false">A4</f>
-        <v>43376</v>
+        <v>43346</v>
       </c>
       <c r="M4" s="0" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="n">
+      <c r="A5" s="5" t="n">
         <f aca="false">A4+1</f>
-        <v>43377</v>
+        <v>43347</v>
       </c>
       <c r="B5" s="3" t="n">
         <f aca="false">A5</f>
-        <v>43377</v>
+        <v>43347</v>
       </c>
       <c r="M5" s="0" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="n">
+      <c r="A6" s="5" t="n">
         <f aca="false">A5+1</f>
-        <v>43378</v>
+        <v>43348</v>
       </c>
       <c r="B6" s="3" t="n">
         <f aca="false">A6</f>
-        <v>43378</v>
+        <v>43348</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="n">
+      <c r="A7" s="5" t="n">
         <f aca="false">A6+1</f>
-        <v>43379</v>
+        <v>43349</v>
       </c>
       <c r="B7" s="3" t="n">
         <f aca="false">A7</f>
-        <v>43379</v>
+        <v>43349</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>19</v>
@@ -1537,13 +1543,13 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="n">
+      <c r="A8" s="5" t="n">
         <f aca="false">A7+1</f>
-        <v>43380</v>
+        <v>43350</v>
       </c>
       <c r="B8" s="3" t="n">
         <f aca="false">A8</f>
-        <v>43380</v>
+        <v>43350</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>19</v>
@@ -1559,13 +1565,13 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="n">
+      <c r="A9" s="5" t="n">
         <f aca="false">A8+1</f>
-        <v>43381</v>
+        <v>43351</v>
       </c>
       <c r="B9" s="3" t="n">
         <f aca="false">A9</f>
-        <v>43381</v>
+        <v>43351</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>19</v>
@@ -1584,13 +1590,13 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="n">
+      <c r="A10" s="5" t="n">
         <f aca="false">A9+1</f>
-        <v>43382</v>
+        <v>43352</v>
       </c>
       <c r="B10" s="3" t="n">
         <f aca="false">A10</f>
-        <v>43382</v>
+        <v>43352</v>
       </c>
       <c r="N10" s="0" t="s">
         <v>19</v>
@@ -1600,13 +1606,13 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="n">
+      <c r="A11" s="5" t="n">
         <f aca="false">A10+1</f>
-        <v>43383</v>
+        <v>43353</v>
       </c>
       <c r="B11" s="3" t="n">
         <f aca="false">A11</f>
-        <v>43383</v>
+        <v>43353</v>
       </c>
       <c r="H11" s="0" t="s">
         <v>21</v>
@@ -1616,23 +1622,23 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="n">
+      <c r="A12" s="5" t="n">
         <f aca="false">A11+1</f>
-        <v>43384</v>
+        <v>43354</v>
       </c>
       <c r="B12" s="3" t="n">
         <f aca="false">A12</f>
-        <v>43384</v>
+        <v>43354</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="n">
+      <c r="A13" s="5" t="n">
         <f aca="false">A12+1</f>
-        <v>43385</v>
+        <v>43355</v>
       </c>
       <c r="B13" s="3" t="n">
         <f aca="false">A13</f>
-        <v>43385</v>
+        <v>43355</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>18</v>
@@ -1645,26 +1651,26 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="n">
+      <c r="A14" s="5" t="n">
         <f aca="false">A13+1</f>
-        <v>43386</v>
+        <v>43356</v>
       </c>
       <c r="B14" s="3" t="n">
         <f aca="false">A14</f>
-        <v>43386</v>
+        <v>43356</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="n">
+      <c r="A15" s="5" t="n">
         <f aca="false">A14+1</f>
-        <v>43387</v>
+        <v>43357</v>
       </c>
       <c r="B15" s="3" t="n">
         <f aca="false">A15</f>
-        <v>43387</v>
+        <v>43357</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>18</v>
@@ -1677,13 +1683,13 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="n">
+      <c r="A16" s="5" t="n">
         <f aca="false">A15+1</f>
-        <v>43388</v>
+        <v>43358</v>
       </c>
       <c r="B16" s="3" t="n">
         <f aca="false">A16</f>
-        <v>43388</v>
+        <v>43358</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>18</v>
@@ -1696,13 +1702,13 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2" t="n">
+      <c r="A17" s="5" t="n">
         <f aca="false">A16+1</f>
-        <v>43389</v>
+        <v>43359</v>
       </c>
       <c r="B17" s="3" t="n">
         <f aca="false">A17</f>
-        <v>43389</v>
+        <v>43359</v>
       </c>
       <c r="O17" s="0" t="s">
         <v>21</v>
@@ -1712,13 +1718,13 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2" t="n">
+      <c r="A18" s="5" t="n">
         <f aca="false">A17+1</f>
-        <v>43390</v>
+        <v>43360</v>
       </c>
       <c r="B18" s="3" t="n">
         <f aca="false">A18</f>
-        <v>43390</v>
+        <v>43360</v>
       </c>
       <c r="F18" s="0" t="s">
         <v>20</v>
@@ -1731,13 +1737,13 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="n">
+      <c r="A19" s="5" t="n">
         <f aca="false">A18+1</f>
-        <v>43391</v>
+        <v>43361</v>
       </c>
       <c r="B19" s="3" t="n">
         <f aca="false">A19</f>
-        <v>43391</v>
+        <v>43361</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>23</v>
@@ -1747,13 +1753,13 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2" t="n">
+      <c r="A20" s="5" t="n">
         <f aca="false">A19+1</f>
-        <v>43392</v>
+        <v>43362</v>
       </c>
       <c r="B20" s="3" t="n">
         <f aca="false">A20</f>
-        <v>43392</v>
+        <v>43362</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>23</v>
@@ -1766,13 +1772,13 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2" t="n">
+      <c r="A21" s="5" t="n">
         <f aca="false">A20+1</f>
-        <v>43393</v>
+        <v>43363</v>
       </c>
       <c r="B21" s="3" t="n">
         <f aca="false">A21</f>
-        <v>43393</v>
+        <v>43363</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>23</v>
@@ -1785,13 +1791,13 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2" t="n">
+      <c r="A22" s="5" t="n">
         <f aca="false">A21+1</f>
-        <v>43394</v>
+        <v>43364</v>
       </c>
       <c r="B22" s="3" t="n">
         <f aca="false">A22</f>
-        <v>43394</v>
+        <v>43364</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>23</v>
@@ -1804,13 +1810,13 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="2" t="n">
+      <c r="A23" s="5" t="n">
         <f aca="false">A22+1</f>
-        <v>43395</v>
+        <v>43365</v>
       </c>
       <c r="B23" s="3" t="n">
         <f aca="false">A23</f>
-        <v>43395</v>
+        <v>43365</v>
       </c>
       <c r="I23" s="0" t="s">
         <v>20</v>
@@ -1820,13 +1826,13 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="2" t="n">
+      <c r="A24" s="5" t="n">
         <f aca="false">A23+1</f>
-        <v>43396</v>
+        <v>43366</v>
       </c>
       <c r="B24" s="3" t="n">
         <f aca="false">A24</f>
-        <v>43396</v>
+        <v>43366</v>
       </c>
       <c r="L24" s="4" t="s">
         <v>23</v>
@@ -1839,13 +1845,13 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="2" t="n">
+      <c r="A25" s="5" t="n">
         <f aca="false">A24+1</f>
-        <v>43397</v>
+        <v>43367</v>
       </c>
       <c r="B25" s="3" t="n">
         <f aca="false">A25</f>
-        <v>43397</v>
+        <v>43367</v>
       </c>
       <c r="L25" s="4" t="s">
         <v>23</v>
@@ -1855,13 +1861,13 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="2" t="n">
+      <c r="A26" s="5" t="n">
         <f aca="false">A25+1</f>
-        <v>43398</v>
+        <v>43368</v>
       </c>
       <c r="B26" s="3" t="n">
         <f aca="false">A26</f>
-        <v>43398</v>
+        <v>43368</v>
       </c>
       <c r="L26" s="4" t="s">
         <v>23</v>
@@ -1871,13 +1877,13 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="2" t="n">
+      <c r="A27" s="5" t="n">
         <f aca="false">A26+1</f>
-        <v>43399</v>
+        <v>43369</v>
       </c>
       <c r="B27" s="3" t="n">
         <f aca="false">A27</f>
-        <v>43399</v>
+        <v>43369</v>
       </c>
       <c r="L27" s="4" t="s">
         <v>23</v>
@@ -1887,13 +1893,13 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="2" t="n">
+      <c r="A28" s="5" t="n">
         <f aca="false">A27+1</f>
-        <v>43400</v>
+        <v>43370</v>
       </c>
       <c r="B28" s="3" t="n">
         <f aca="false">A28</f>
-        <v>43400</v>
+        <v>43370</v>
       </c>
       <c r="L28" s="4" t="s">
         <v>23</v>
@@ -1903,46 +1909,46 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="2" t="n">
+      <c r="A29" s="5" t="n">
         <f aca="false">A28+1</f>
-        <v>43401</v>
+        <v>43371</v>
       </c>
       <c r="B29" s="3" t="n">
         <f aca="false">A29</f>
-        <v>43401</v>
+        <v>43371</v>
       </c>
       <c r="L29" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="2" t="n">
+      <c r="A30" s="5" t="n">
         <f aca="false">A29+1</f>
-        <v>43402</v>
+        <v>43372</v>
       </c>
       <c r="B30" s="3" t="n">
         <f aca="false">A30</f>
-        <v>43402</v>
+        <v>43372</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="2" t="n">
+      <c r="A31" s="5" t="n">
         <f aca="false">A30+1</f>
-        <v>43403</v>
+        <v>43373</v>
       </c>
       <c r="B31" s="3" t="n">
         <f aca="false">A31</f>
-        <v>43403</v>
+        <v>43373</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="2" t="n">
+      <c r="A32" s="5" t="n">
         <f aca="false">A31+1</f>
-        <v>43404</v>
+        <v>43374</v>
       </c>
       <c r="B32" s="3" t="n">
         <f aca="false">A32</f>
-        <v>43404</v>
+        <v>43374</v>
       </c>
     </row>
   </sheetData>
@@ -1963,8 +1969,8 @@
   </sheetPr>
   <dimension ref="A1:U32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2033,7 +2039,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="n">
+      <c r="A2" s="5" t="n">
         <v>43374</v>
       </c>
       <c r="B2" s="3" t="n">
@@ -2042,7 +2048,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="n">
+      <c r="A3" s="5" t="n">
         <f aca="false">A2+1</f>
         <v>43375</v>
       </c>
@@ -2055,7 +2061,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="n">
+      <c r="A4" s="5" t="n">
         <f aca="false">A3+1</f>
         <v>43376</v>
       </c>
@@ -2068,7 +2074,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="n">
+      <c r="A5" s="5" t="n">
         <f aca="false">A4+1</f>
         <v>43377</v>
       </c>
@@ -2081,7 +2087,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="n">
+      <c r="A6" s="5" t="n">
         <f aca="false">A5+1</f>
         <v>43378</v>
       </c>
@@ -2094,7 +2100,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="n">
+      <c r="A7" s="5" t="n">
         <f aca="false">A6+1</f>
         <v>43379</v>
       </c>
@@ -2110,7 +2116,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="n">
+      <c r="A8" s="5" t="n">
         <f aca="false">A7+1</f>
         <v>43380</v>
       </c>
@@ -2132,7 +2138,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="n">
+      <c r="A9" s="5" t="n">
         <f aca="false">A8+1</f>
         <v>43381</v>
       </c>
@@ -2157,7 +2163,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="n">
+      <c r="A10" s="5" t="n">
         <f aca="false">A9+1</f>
         <v>43382</v>
       </c>
@@ -2173,7 +2179,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="n">
+      <c r="A11" s="5" t="n">
         <f aca="false">A10+1</f>
         <v>43383</v>
       </c>
@@ -2189,7 +2195,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="n">
+      <c r="A12" s="5" t="n">
         <f aca="false">A11+1</f>
         <v>43384</v>
       </c>
@@ -2199,7 +2205,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="n">
+      <c r="A13" s="5" t="n">
         <f aca="false">A12+1</f>
         <v>43385</v>
       </c>
@@ -2218,7 +2224,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="n">
+      <c r="A14" s="5" t="n">
         <f aca="false">A13+1</f>
         <v>43386</v>
       </c>
@@ -2231,7 +2237,7 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="n">
+      <c r="A15" s="5" t="n">
         <f aca="false">A14+1</f>
         <v>43387</v>
       </c>
@@ -2250,7 +2256,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="n">
+      <c r="A16" s="5" t="n">
         <f aca="false">A15+1</f>
         <v>43388</v>
       </c>
@@ -2269,7 +2275,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2" t="n">
+      <c r="A17" s="5" t="n">
         <f aca="false">A16+1</f>
         <v>43389</v>
       </c>
@@ -2288,7 +2294,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2" t="n">
+      <c r="A18" s="5" t="n">
         <f aca="false">A17+1</f>
         <v>43390</v>
       </c>
@@ -2310,7 +2316,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="n">
+      <c r="A19" s="5" t="n">
         <f aca="false">A18+1</f>
         <v>43391</v>
       </c>
@@ -2332,7 +2338,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2" t="n">
+      <c r="A20" s="5" t="n">
         <f aca="false">A19+1</f>
         <v>43392</v>
       </c>
@@ -2357,7 +2363,7 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2" t="n">
+      <c r="A21" s="5" t="n">
         <f aca="false">A20+1</f>
         <v>43393</v>
       </c>
@@ -2382,7 +2388,7 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2" t="n">
+      <c r="A22" s="5" t="n">
         <f aca="false">A21+1</f>
         <v>43394</v>
       </c>
@@ -2407,7 +2413,7 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="2" t="n">
+      <c r="A23" s="5" t="n">
         <f aca="false">A22+1</f>
         <v>43395</v>
       </c>
@@ -2429,7 +2435,7 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="2" t="n">
+      <c r="A24" s="5" t="n">
         <f aca="false">A23+1</f>
         <v>43396</v>
       </c>
@@ -2448,7 +2454,7 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="2" t="n">
+      <c r="A25" s="5" t="n">
         <f aca="false">A24+1</f>
         <v>43397</v>
       </c>
@@ -2464,7 +2470,7 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="2" t="n">
+      <c r="A26" s="5" t="n">
         <f aca="false">A25+1</f>
         <v>43398</v>
       </c>
@@ -2480,7 +2486,7 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="2" t="n">
+      <c r="A27" s="5" t="n">
         <f aca="false">A26+1</f>
         <v>43399</v>
       </c>
@@ -2496,7 +2502,7 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="2" t="n">
+      <c r="A28" s="5" t="n">
         <f aca="false">A27+1</f>
         <v>43400</v>
       </c>
@@ -2512,7 +2518,7 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="2" t="n">
+      <c r="A29" s="5" t="n">
         <f aca="false">A28+1</f>
         <v>43401</v>
       </c>
@@ -2525,7 +2531,7 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="2" t="n">
+      <c r="A30" s="5" t="n">
         <f aca="false">A29+1</f>
         <v>43402</v>
       </c>
@@ -2535,7 +2541,7 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="2" t="n">
+      <c r="A31" s="5" t="n">
         <f aca="false">A30+1</f>
         <v>43403</v>
       </c>
@@ -2545,7 +2551,7 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="2" t="n">
+      <c r="A32" s="5" t="n">
         <f aca="false">A31+1</f>
         <v>43404</v>
       </c>
@@ -2570,9 +2576,618 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:U32"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.45"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="n">
+        <v>43405</v>
+      </c>
+      <c r="B2" s="3" t="n">
+        <f aca="false">A2</f>
+        <v>43405</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="n">
+        <f aca="false">A2+1</f>
+        <v>43406</v>
+      </c>
+      <c r="B3" s="3" t="n">
+        <f aca="false">A3</f>
+        <v>43406</v>
+      </c>
+      <c r="M3" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="n">
+        <f aca="false">A3+1</f>
+        <v>43407</v>
+      </c>
+      <c r="B4" s="3" t="n">
+        <f aca="false">A4</f>
+        <v>43407</v>
+      </c>
+      <c r="M4" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="n">
+        <f aca="false">A4+1</f>
+        <v>43408</v>
+      </c>
+      <c r="B5" s="3" t="n">
+        <f aca="false">A5</f>
+        <v>43408</v>
+      </c>
+      <c r="M5" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="n">
+        <f aca="false">A5+1</f>
+        <v>43409</v>
+      </c>
+      <c r="B6" s="3" t="n">
+        <f aca="false">A6</f>
+        <v>43409</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="n">
+        <f aca="false">A6+1</f>
+        <v>43410</v>
+      </c>
+      <c r="B7" s="3" t="n">
+        <f aca="false">A7</f>
+        <v>43410</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="O7" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="n">
+        <f aca="false">A7+1</f>
+        <v>43411</v>
+      </c>
+      <c r="B8" s="3" t="n">
+        <f aca="false">A8</f>
+        <v>43411</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="O8" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q8" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="n">
+        <f aca="false">A8+1</f>
+        <v>43412</v>
+      </c>
+      <c r="B9" s="3" t="n">
+        <f aca="false">A9</f>
+        <v>43412</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="N9" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="O9" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q9" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="n">
+        <f aca="false">A9+1</f>
+        <v>43413</v>
+      </c>
+      <c r="B10" s="3" t="n">
+        <f aca="false">A10</f>
+        <v>43413</v>
+      </c>
+      <c r="N10" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q10" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="n">
+        <f aca="false">A10+1</f>
+        <v>43414</v>
+      </c>
+      <c r="B11" s="3" t="n">
+        <f aca="false">A11</f>
+        <v>43414</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="P11" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="n">
+        <f aca="false">A11+1</f>
+        <v>43415</v>
+      </c>
+      <c r="B12" s="3" t="n">
+        <f aca="false">A12</f>
+        <v>43415</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="n">
+        <f aca="false">A12+1</f>
+        <v>43416</v>
+      </c>
+      <c r="B13" s="3" t="n">
+        <f aca="false">A13</f>
+        <v>43416</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="I13" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="P13" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="5" t="n">
+        <f aca="false">A13+1</f>
+        <v>43417</v>
+      </c>
+      <c r="B14" s="3" t="n">
+        <f aca="false">A14</f>
+        <v>43417</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5" t="n">
+        <f aca="false">A14+1</f>
+        <v>43418</v>
+      </c>
+      <c r="B15" s="3" t="n">
+        <f aca="false">A15</f>
+        <v>43418</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="O15" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="R15" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="5" t="n">
+        <f aca="false">A15+1</f>
+        <v>43419</v>
+      </c>
+      <c r="B16" s="3" t="n">
+        <f aca="false">A16</f>
+        <v>43419</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="O16" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="R16" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="5" t="n">
+        <f aca="false">A16+1</f>
+        <v>43420</v>
+      </c>
+      <c r="B17" s="3" t="n">
+        <f aca="false">A17</f>
+        <v>43420</v>
+      </c>
+      <c r="M17" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O17" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="R17" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="5" t="n">
+        <f aca="false">A17+1</f>
+        <v>43421</v>
+      </c>
+      <c r="B18" s="3" t="n">
+        <f aca="false">A18</f>
+        <v>43421</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K18" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="R18" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="5" t="n">
+        <f aca="false">A18+1</f>
+        <v>43422</v>
+      </c>
+      <c r="B19" s="3" t="n">
+        <f aca="false">A19</f>
+        <v>43422</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="M19" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="5" t="n">
+        <f aca="false">A19+1</f>
+        <v>43423</v>
+      </c>
+      <c r="B20" s="3" t="n">
+        <f aca="false">A20</f>
+        <v>43423</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="M20" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P20" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="5" t="n">
+        <f aca="false">A20+1</f>
+        <v>43424</v>
+      </c>
+      <c r="B21" s="3" t="n">
+        <f aca="false">A21</f>
+        <v>43424</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O21" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="P21" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="U21" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="5" t="n">
+        <f aca="false">A21+1</f>
+        <v>43425</v>
+      </c>
+      <c r="B22" s="3" t="n">
+        <f aca="false">A22</f>
+        <v>43425</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I22" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="O22" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="U22" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="5" t="n">
+        <f aca="false">A22+1</f>
+        <v>43426</v>
+      </c>
+      <c r="B23" s="3" t="n">
+        <f aca="false">A23</f>
+        <v>43426</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I23" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="O23" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="U23" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="5" t="n">
+        <f aca="false">A23+1</f>
+        <v>43427</v>
+      </c>
+      <c r="B24" s="3" t="n">
+        <f aca="false">A24</f>
+        <v>43427</v>
+      </c>
+      <c r="L24" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O24" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="S24" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="5" t="n">
+        <f aca="false">A24+1</f>
+        <v>43428</v>
+      </c>
+      <c r="B25" s="3" t="n">
+        <f aca="false">A25</f>
+        <v>43428</v>
+      </c>
+      <c r="L25" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="S25" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="5" t="n">
+        <f aca="false">A25+1</f>
+        <v>43429</v>
+      </c>
+      <c r="B26" s="3" t="n">
+        <f aca="false">A26</f>
+        <v>43429</v>
+      </c>
+      <c r="L26" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="S26" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="5" t="n">
+        <f aca="false">A26+1</f>
+        <v>43430</v>
+      </c>
+      <c r="B27" s="3" t="n">
+        <f aca="false">A27</f>
+        <v>43430</v>
+      </c>
+      <c r="L27" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="S27" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="5" t="n">
+        <f aca="false">A27+1</f>
+        <v>43431</v>
+      </c>
+      <c r="B28" s="3" t="n">
+        <f aca="false">A28</f>
+        <v>43431</v>
+      </c>
+      <c r="L28" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="S28" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="5" t="n">
+        <f aca="false">A28+1</f>
+        <v>43432</v>
+      </c>
+      <c r="B29" s="3" t="n">
+        <f aca="false">A29</f>
+        <v>43432</v>
+      </c>
+      <c r="L29" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="5" t="n">
+        <f aca="false">A29+1</f>
+        <v>43433</v>
+      </c>
+      <c r="B30" s="3" t="n">
+        <f aca="false">A30</f>
+        <v>43433</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="5" t="n">
+        <f aca="false">A30+1</f>
+        <v>43434</v>
+      </c>
+      <c r="B31" s="3" t="n">
+        <f aca="false">A31</f>
+        <v>43434</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="5" t="n">
+        <f aca="false">A31+1</f>
+        <v>43435</v>
+      </c>
+      <c r="B32" s="3" t="n">
+        <f aca="false">A32</f>
+        <v>43435</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -2739,7 +3354,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -2986,7 +3601,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>

</xml_diff>